<commit_message>
New versions of the model
</commit_message>
<xml_diff>
--- a/inflation_forecast.xlsx
+++ b/inflation_forecast.xlsx
@@ -3107,7 +3107,7 @@
         <v>44834</v>
       </c>
       <c r="B334" t="n">
-        <v>0.4675619685649872</v>
+        <v>0.9599317154288292</v>
       </c>
     </row>
     <row r="335">
@@ -3115,7 +3115,7 @@
         <v>44865</v>
       </c>
       <c r="B335" t="n">
-        <v>0.3068162712454796</v>
+        <v>0.9455632781237364</v>
       </c>
     </row>
     <row r="336">
@@ -3123,7 +3123,7 @@
         <v>44895</v>
       </c>
       <c r="B336" t="n">
-        <v>0.6163384962081909</v>
+        <v>0.7641119734942913</v>
       </c>
     </row>
     <row r="337">
@@ -3131,7 +3131,7 @@
         <v>44926</v>
       </c>
       <c r="B337" t="n">
-        <v>1.318009146973491</v>
+        <v>1.164684123396873</v>
       </c>
     </row>
     <row r="338">
@@ -3139,7 +3139,7 @@
         <v>44957</v>
       </c>
       <c r="B338" t="n">
-        <v>0.8235102917253971</v>
+        <v>1.156321626976132</v>
       </c>
     </row>
     <row r="339">
@@ -3147,7 +3147,7 @@
         <v>44985</v>
       </c>
       <c r="B339" t="n">
-        <v>0.7006764157116413</v>
+        <v>0.9391011016070843</v>
       </c>
     </row>
     <row r="340">
@@ -3155,7 +3155,7 @@
         <v>45016</v>
       </c>
       <c r="B340" t="n">
-        <v>0.9234849925339222</v>
+        <v>0.6331674814224243</v>
       </c>
     </row>
     <row r="341">
@@ -3163,7 +3163,7 @@
         <v>45046</v>
       </c>
       <c r="B341" t="n">
-        <v>1.022161024808884</v>
+        <v>0.5372912478446961</v>
       </c>
     </row>
     <row r="342">
@@ -3171,7 +3171,7 @@
         <v>45077</v>
       </c>
       <c r="B342" t="n">
-        <v>1.522321152240038</v>
+        <v>0.7946128785610199</v>
       </c>
     </row>
     <row r="343">
@@ -3179,7 +3179,7 @@
         <v>45107</v>
       </c>
       <c r="B343" t="n">
-        <v>1.644392207115889</v>
+        <v>0.7913253098726273</v>
       </c>
     </row>
     <row r="344">
@@ -3187,7 +3187,7 @@
         <v>45138</v>
       </c>
       <c r="B344" t="n">
-        <v>0.8894066867232323</v>
+        <v>0.5530621093511582</v>
       </c>
     </row>
     <row r="345">
@@ -3195,7 +3195,7 @@
         <v>45169</v>
       </c>
       <c r="B345" t="n">
-        <v>0.3281771567463875</v>
+        <v>0.4222658997774124</v>
       </c>
     </row>
     <row r="346">
@@ -3203,7 +3203,7 @@
         <v>45199</v>
       </c>
       <c r="B346" t="n">
-        <v>0.3716470205783844</v>
+        <v>0.2527838963270188</v>
       </c>
     </row>
     <row r="347">
@@ -3211,7 +3211,7 @@
         <v>45230</v>
       </c>
       <c r="B347" t="n">
-        <v>1.076871888153255</v>
+        <v>0.4344980749487877</v>
       </c>
     </row>
     <row r="348">
@@ -3219,7 +3219,7 @@
         <v>45260</v>
       </c>
       <c r="B348" t="n">
-        <v>0.3026957115530968</v>
+        <v>0.1481849277019501</v>
       </c>
     </row>
     <row r="349">
@@ -3227,7 +3227,7 @@
         <v>45291</v>
       </c>
       <c r="B349" t="n">
-        <v>0.4600190761685372</v>
+        <v>0.4633985915780067</v>
       </c>
     </row>
     <row r="350">
@@ -3235,7 +3235,7 @@
         <v>45322</v>
       </c>
       <c r="B350" t="n">
-        <v>0.6706969979405403</v>
+        <v>0.5122897350788117</v>
       </c>
     </row>
     <row r="351">
@@ -3243,7 +3243,7 @@
         <v>45351</v>
       </c>
       <c r="B351" t="n">
-        <v>0.3637743192911148</v>
+        <v>0.2426398795843124</v>
       </c>
     </row>
     <row r="352">
@@ -3251,7 +3251,7 @@
         <v>45382</v>
       </c>
       <c r="B352" t="n">
-        <v>0.7005952522158623</v>
+        <v>1.27256611071527</v>
       </c>
     </row>
     <row r="353">
@@ -3259,7 +3259,7 @@
         <v>45412</v>
       </c>
       <c r="B353" t="n">
-        <v>0.2752186858654022</v>
+        <v>1.022898229211569</v>
       </c>
     </row>
     <row r="354">
@@ -3267,7 +3267,7 @@
         <v>45443</v>
       </c>
       <c r="B354" t="n">
-        <v>0.3424363678693771</v>
+        <v>0.1922542336583138</v>
       </c>
     </row>
     <row r="355">
@@ -3275,7 +3275,7 @@
         <v>45473</v>
       </c>
       <c r="B355" t="n">
-        <v>0.2981805384159088</v>
+        <v>0.6728441748023033</v>
       </c>
     </row>
     <row r="356">
@@ -3283,7 +3283,7 @@
         <v>45504</v>
       </c>
       <c r="B356" t="n">
-        <v>0.4294581532478333</v>
+        <v>0.6459268774092197</v>
       </c>
     </row>
     <row r="357">
@@ -3291,7 +3291,7 @@
         <v>45535</v>
       </c>
       <c r="B357" t="n">
-        <v>0.4823932166397571</v>
+        <v>0.5305473661422729</v>
       </c>
     </row>
     <row r="358">
@@ -3299,7 +3299,7 @@
         <v>45565</v>
       </c>
       <c r="B358" t="n">
-        <v>0.408081277012825</v>
+        <v>0.5466447226703167</v>
       </c>
     </row>
     <row r="359">
@@ -3307,7 +3307,7 @@
         <v>45596</v>
       </c>
       <c r="B359" t="n">
-        <v>0.3594385159015656</v>
+        <v>0.3594466164708138</v>
       </c>
     </row>
     <row r="360">
@@ -3315,7 +3315,7 @@
         <v>45626</v>
       </c>
       <c r="B360" t="n">
-        <v>0.5343209689855576</v>
+        <v>0.2048006477952004</v>
       </c>
     </row>
     <row r="361">
@@ -3323,7 +3323,7 @@
         <v>45657</v>
       </c>
       <c r="B361" t="n">
-        <v>0.4718641072511673</v>
+        <v>0.1636517548561096</v>
       </c>
     </row>
     <row r="362">
@@ -3331,7 +3331,7 @@
         <v>45688</v>
       </c>
       <c r="B362" t="n">
-        <v>0.3505756515264511</v>
+        <v>0.8283556419610977</v>
       </c>
     </row>
     <row r="363">
@@ -3339,7 +3339,7 @@
         <v>45716</v>
       </c>
       <c r="B363" t="n">
-        <v>0.4579459090530872</v>
+        <v>0.549017400443554</v>
       </c>
     </row>
     <row r="364">
@@ -3347,7 +3347,7 @@
         <v>45747</v>
       </c>
       <c r="B364" t="n">
-        <v>0.4620160242915153</v>
+        <v>0.0838139119744301</v>
       </c>
     </row>
     <row r="365">
@@ -3355,7 +3355,7 @@
         <v>45777</v>
       </c>
       <c r="B365" t="n">
-        <v>0.3936970856785774</v>
+        <v>0.5645945847034455</v>
       </c>
     </row>
     <row r="366">
@@ -3363,7 +3363,7 @@
         <v>45808</v>
       </c>
       <c r="B366" t="n">
-        <v>0.5495314183831215</v>
+        <v>0.4806778948009014</v>
       </c>
     </row>
     <row r="367">
@@ -3371,7 +3371,7 @@
         <v>45838</v>
       </c>
       <c r="B367" t="n">
-        <v>0.3323291718959808</v>
+        <v>0.2398127809166908</v>
       </c>
     </row>
     <row r="368">
@@ -3379,7 +3379,7 @@
         <v>45869</v>
       </c>
       <c r="B368" t="n">
-        <v>0.330226916372776</v>
+        <v>0.4772502493858338</v>
       </c>
     </row>
     <row r="369">
@@ -3387,7 +3387,7 @@
         <v>45900</v>
       </c>
       <c r="B369" t="n">
-        <v>0.2030036890506745</v>
+        <v>0.3967638349533081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Model with new parameters
</commit_message>
<xml_diff>
--- a/inflation_forecast.xlsx
+++ b/inflation_forecast.xlsx
@@ -3107,7 +3107,7 @@
         <v>44834</v>
       </c>
       <c r="B334" t="n">
-        <v>0.9599317154288292</v>
+        <v>0.8810912419855594</v>
       </c>
     </row>
     <row r="335">
@@ -3115,7 +3115,7 @@
         <v>44865</v>
       </c>
       <c r="B335" t="n">
-        <v>0.9455632781237364</v>
+        <v>0.8214963534474373</v>
       </c>
     </row>
     <row r="336">
@@ -3123,7 +3123,7 @@
         <v>44895</v>
       </c>
       <c r="B336" t="n">
-        <v>0.7641119734942913</v>
+        <v>0.8869845113158226</v>
       </c>
     </row>
     <row r="337">
@@ -3131,7 +3131,7 @@
         <v>44926</v>
       </c>
       <c r="B337" t="n">
-        <v>1.164684123396873</v>
+        <v>0.8105607953667641</v>
       </c>
     </row>
     <row r="338">
@@ -3139,7 +3139,7 @@
         <v>44957</v>
       </c>
       <c r="B338" t="n">
-        <v>1.156321626976132</v>
+        <v>0.7763261064887047</v>
       </c>
     </row>
     <row r="339">
@@ -3147,7 +3147,7 @@
         <v>44985</v>
       </c>
       <c r="B339" t="n">
-        <v>0.9391011016070843</v>
+        <v>1.029825215339661</v>
       </c>
     </row>
     <row r="340">
@@ -3155,7 +3155,7 @@
         <v>45016</v>
       </c>
       <c r="B340" t="n">
-        <v>0.6331674814224243</v>
+        <v>0.7396623514592647</v>
       </c>
     </row>
     <row r="341">
@@ -3163,7 +3163,7 @@
         <v>45046</v>
       </c>
       <c r="B341" t="n">
-        <v>0.5372912478446961</v>
+        <v>0.9300873246788979</v>
       </c>
     </row>
     <row r="342">
@@ -3171,7 +3171,7 @@
         <v>45077</v>
       </c>
       <c r="B342" t="n">
-        <v>0.7946128785610199</v>
+        <v>0.7431439656019211</v>
       </c>
     </row>
     <row r="343">
@@ -3179,7 +3179,7 @@
         <v>45107</v>
       </c>
       <c r="B343" t="n">
-        <v>0.7913253098726273</v>
+        <v>1.252684499621391</v>
       </c>
     </row>
     <row r="344">
@@ -3187,7 +3187,7 @@
         <v>45138</v>
       </c>
       <c r="B344" t="n">
-        <v>0.5530621093511582</v>
+        <v>0.5400192460417748</v>
       </c>
     </row>
     <row r="345">
@@ -3195,7 +3195,7 @@
         <v>45169</v>
       </c>
       <c r="B345" t="n">
-        <v>0.4222658997774124</v>
+        <v>0.4820150673389435</v>
       </c>
     </row>
     <row r="346">
@@ -3203,7 +3203,7 @@
         <v>45199</v>
       </c>
       <c r="B346" t="n">
-        <v>0.2527838963270188</v>
+        <v>0.102651838362217</v>
       </c>
     </row>
     <row r="347">
@@ -3211,7 +3211,7 @@
         <v>45230</v>
       </c>
       <c r="B347" t="n">
-        <v>0.4344980749487877</v>
+        <v>0.5836758437752724</v>
       </c>
     </row>
     <row r="348">
@@ -3219,7 +3219,7 @@
         <v>45260</v>
       </c>
       <c r="B348" t="n">
-        <v>0.1481849277019501</v>
+        <v>0.3101505497097969</v>
       </c>
     </row>
     <row r="349">
@@ -3227,7 +3227,7 @@
         <v>45291</v>
       </c>
       <c r="B349" t="n">
-        <v>0.4633985915780067</v>
+        <v>0.4494251096248627</v>
       </c>
     </row>
     <row r="350">
@@ -3235,7 +3235,7 @@
         <v>45322</v>
       </c>
       <c r="B350" t="n">
-        <v>0.5122897350788117</v>
+        <v>0.3493212205171585</v>
       </c>
     </row>
     <row r="351">
@@ -3243,7 +3243,7 @@
         <v>45351</v>
       </c>
       <c r="B351" t="n">
-        <v>0.2426398795843124</v>
+        <v>-0.07923666030168532</v>
       </c>
     </row>
     <row r="352">
@@ -3251,7 +3251,7 @@
         <v>45382</v>
       </c>
       <c r="B352" t="n">
-        <v>1.27256611071527</v>
+        <v>1.01478587731719</v>
       </c>
     </row>
     <row r="353">
@@ -3259,7 +3259,7 @@
         <v>45412</v>
       </c>
       <c r="B353" t="n">
-        <v>1.022898229211569</v>
+        <v>0.3373434242606163</v>
       </c>
     </row>
     <row r="354">
@@ -3267,7 +3267,7 @@
         <v>45443</v>
       </c>
       <c r="B354" t="n">
-        <v>0.1922542336583138</v>
+        <v>0.580757271796465</v>
       </c>
     </row>
     <row r="355">
@@ -3275,7 +3275,7 @@
         <v>45473</v>
       </c>
       <c r="B355" t="n">
-        <v>0.6728441748023033</v>
+        <v>0.05624767482280732</v>
       </c>
     </row>
     <row r="356">
@@ -3283,7 +3283,7 @@
         <v>45504</v>
       </c>
       <c r="B356" t="n">
-        <v>0.6459268774092197</v>
+        <v>0.3945392292737961</v>
       </c>
     </row>
     <row r="357">
@@ -3291,7 +3291,7 @@
         <v>45535</v>
       </c>
       <c r="B357" t="n">
-        <v>0.5305473661422729</v>
+        <v>0.4908187028765679</v>
       </c>
     </row>
     <row r="358">
@@ -3299,7 +3299,7 @@
         <v>45565</v>
       </c>
       <c r="B358" t="n">
-        <v>0.5466447226703167</v>
+        <v>0.4117062291502953</v>
       </c>
     </row>
     <row r="359">
@@ -3307,7 +3307,7 @@
         <v>45596</v>
       </c>
       <c r="B359" t="n">
-        <v>0.3594466164708138</v>
+        <v>0.3670210695266723</v>
       </c>
     </row>
     <row r="360">
@@ -3315,7 +3315,7 @@
         <v>45626</v>
       </c>
       <c r="B360" t="n">
-        <v>0.2048006477952004</v>
+        <v>-0.2127494010329246</v>
       </c>
     </row>
     <row r="361">
@@ -3323,7 +3323,7 @@
         <v>45657</v>
       </c>
       <c r="B361" t="n">
-        <v>0.1636517548561096</v>
+        <v>0.3056404262781143</v>
       </c>
     </row>
     <row r="362">
@@ -3331,7 +3331,7 @@
         <v>45688</v>
       </c>
       <c r="B362" t="n">
-        <v>0.8283556419610977</v>
+        <v>0.9879850387573242</v>
       </c>
     </row>
     <row r="363">
@@ -3339,7 +3339,7 @@
         <v>45716</v>
       </c>
       <c r="B363" t="n">
-        <v>0.549017400443554</v>
+        <v>0.4814973147213459</v>
       </c>
     </row>
     <row r="364">
@@ -3347,7 +3347,7 @@
         <v>45747</v>
       </c>
       <c r="B364" t="n">
-        <v>0.0838139119744301</v>
+        <v>0.3756522786617279</v>
       </c>
     </row>
     <row r="365">
@@ -3355,7 +3355,7 @@
         <v>45777</v>
       </c>
       <c r="B365" t="n">
-        <v>0.5645945847034455</v>
+        <v>0.8622520268708468</v>
       </c>
     </row>
     <row r="366">
@@ -3363,7 +3363,7 @@
         <v>45808</v>
       </c>
       <c r="B366" t="n">
-        <v>0.4806778948009014</v>
+        <v>0.4422421139478683</v>
       </c>
     </row>
     <row r="367">
@@ -3371,7 +3371,7 @@
         <v>45838</v>
       </c>
       <c r="B367" t="n">
-        <v>0.2398127809166908</v>
+        <v>0.3255287966132164</v>
       </c>
     </row>
     <row r="368">
@@ -3379,7 +3379,7 @@
         <v>45869</v>
       </c>
       <c r="B368" t="n">
-        <v>0.4772502493858338</v>
+        <v>0.2913089412450791</v>
       </c>
     </row>
     <row r="369">
@@ -3387,7 +3387,7 @@
         <v>45900</v>
       </c>
       <c r="B369" t="n">
-        <v>0.3967638349533081</v>
+        <v>0.1962499183416367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>